<commit_message>
added multiple data class
</commit_message>
<xml_diff>
--- a/test_data/WriteData.xlsx
+++ b/test_data/WriteData.xlsx
@@ -6,15 +6,39 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tech" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>EmpID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
   <si>
     <t>Tech Global</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>Ulan</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Abe</t>
+  </si>
+  <si>
+    <t>Instructor</t>
   </si>
 </sst>
 </file>
@@ -59,15 +83,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>101.0</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>